<commit_message>
✨Feat : CrimeZone Loader
</commit_message>
<xml_diff>
--- a/Documents/CrimePoint_within3km.xlsx
+++ b/Documents/CrimePoint_within3km.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimdoo-young/#ConnectFolder/#Project/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seojiung/Documents/GitHub/DisabilityCrimeNavigator/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED9DE57-8543-944D-8434-5146F486CC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA9E86F-CEB3-6D4E-9982-42CE86C7A7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" xr2:uid="{53916054-8B8C-4E74-BC5F-10B546F4D0E4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{53916054-8B8C-4E74-BC5F-10B546F4D0E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -56,30 +56,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>강도</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>127.43016543288326 </t>
   </si>
   <si>
-    <t>살인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Robbery</t>
   </si>
   <si>
-    <t>성폭력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Murder</t>
   </si>
   <si>
-    <t>폭력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Sexual_Violence</t>
   </si>
   <si>
-    <t>127.43016543288326 </t>
+    <t>Violence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +96,12 @@
       <color rgb="FF424242"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFC77DBB"/>
+      <name val="JetBrains Mono"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,11 +126,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -447,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E8108C-04BD-2A42-96C4-40717F420405}">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -480,8 +485,8 @@
       <c r="C2">
         <v>100</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -497,8 +502,8 @@
       <c r="C3">
         <v>32</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -514,8 +519,8 @@
       <c r="C4">
         <v>35</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -531,8 +536,8 @@
       <c r="C5">
         <v>35</v>
       </c>
-      <c r="D5" t="s">
-        <v>5</v>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -548,8 +553,8 @@
       <c r="C6">
         <v>40</v>
       </c>
-      <c r="D6" t="s">
-        <v>5</v>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -565,8 +570,8 @@
       <c r="C7">
         <v>40</v>
       </c>
-      <c r="D7" t="s">
-        <v>5</v>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -582,8 +587,8 @@
       <c r="C8">
         <v>50</v>
       </c>
-      <c r="D8" t="s">
-        <v>5</v>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -599,8 +604,8 @@
       <c r="C9">
         <v>50</v>
       </c>
-      <c r="D9" t="s">
-        <v>5</v>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -616,8 +621,8 @@
       <c r="C10">
         <v>100</v>
       </c>
-      <c r="D10" t="s">
-        <v>5</v>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -633,8 +638,8 @@
       <c r="C11">
         <v>110</v>
       </c>
-      <c r="D11" t="s">
-        <v>6</v>
+      <c r="D11" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -650,8 +655,8 @@
       <c r="C12">
         <v>130</v>
       </c>
-      <c r="D12" t="s">
-        <v>6</v>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -667,8 +672,8 @@
       <c r="C13">
         <v>130</v>
       </c>
-      <c r="D13" t="s">
-        <v>6</v>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -684,8 +689,8 @@
       <c r="C14">
         <v>100</v>
       </c>
-      <c r="D14" t="s">
-        <v>7</v>
+      <c r="D14" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -701,8 +706,8 @@
       <c r="C15">
         <v>120</v>
       </c>
-      <c r="D15" t="s">
-        <v>7</v>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E15">
         <v>3</v>
@@ -718,8 +723,8 @@
       <c r="C16">
         <v>85</v>
       </c>
-      <c r="D16" t="s">
-        <v>7</v>
+      <c r="D16" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -735,8 +740,8 @@
       <c r="C17">
         <v>100</v>
       </c>
-      <c r="D17" t="s">
-        <v>7</v>
+      <c r="D17" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -752,8 +757,8 @@
       <c r="C18">
         <v>100</v>
       </c>
-      <c r="D18" t="s">
-        <v>7</v>
+      <c r="D18" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -769,8 +774,8 @@
       <c r="C19">
         <v>80</v>
       </c>
-      <c r="D19" t="s">
-        <v>7</v>
+      <c r="D19" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E19">
         <v>3</v>
@@ -786,8 +791,8 @@
       <c r="C20">
         <v>60</v>
       </c>
-      <c r="D20" t="s">
-        <v>7</v>
+      <c r="D20" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E20">
         <v>3</v>
@@ -803,8 +808,8 @@
       <c r="C21">
         <v>90</v>
       </c>
-      <c r="D21" t="s">
-        <v>7</v>
+      <c r="D21" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E21">
         <v>3</v>
@@ -820,8 +825,8 @@
       <c r="C22">
         <v>100</v>
       </c>
-      <c r="D22" t="s">
-        <v>7</v>
+      <c r="D22" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E22">
         <v>3</v>
@@ -837,8 +842,8 @@
       <c r="C23">
         <v>100</v>
       </c>
-      <c r="D23" t="s">
-        <v>7</v>
+      <c r="D23" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E23">
         <v>3</v>
@@ -854,8 +859,8 @@
       <c r="C24">
         <v>120</v>
       </c>
-      <c r="D24" t="s">
-        <v>7</v>
+      <c r="D24" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -871,8 +876,8 @@
       <c r="C25">
         <v>100</v>
       </c>
-      <c r="D25" t="s">
-        <v>7</v>
+      <c r="D25" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E25">
         <v>3</v>
@@ -888,8 +893,8 @@
       <c r="C26">
         <v>85</v>
       </c>
-      <c r="D26" t="s">
-        <v>7</v>
+      <c r="D26" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E26">
         <v>3</v>
@@ -905,8 +910,8 @@
       <c r="C27">
         <v>100</v>
       </c>
-      <c r="D27" t="s">
-        <v>7</v>
+      <c r="D27" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E27">
         <v>3</v>
@@ -922,8 +927,8 @@
       <c r="C28">
         <v>50</v>
       </c>
-      <c r="D28" t="s">
-        <v>7</v>
+      <c r="D28" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E28">
         <v>2</v>
@@ -939,8 +944,8 @@
       <c r="C29">
         <v>40</v>
       </c>
-      <c r="D29" t="s">
-        <v>7</v>
+      <c r="D29" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -956,8 +961,8 @@
       <c r="C30">
         <v>85</v>
       </c>
-      <c r="D30" t="s">
-        <v>7</v>
+      <c r="D30" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E30">
         <v>3</v>
@@ -973,8 +978,8 @@
       <c r="C31">
         <v>100</v>
       </c>
-      <c r="D31" t="s">
-        <v>7</v>
+      <c r="D31" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E31">
         <v>3</v>
@@ -990,8 +995,8 @@
       <c r="C32">
         <v>70</v>
       </c>
-      <c r="D32" t="s">
-        <v>7</v>
+      <c r="D32" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -1007,8 +1012,8 @@
       <c r="C33">
         <v>75</v>
       </c>
-      <c r="D33" t="s">
-        <v>7</v>
+      <c r="D33" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E33">
         <v>3</v>
@@ -1024,8 +1029,8 @@
       <c r="C34">
         <v>200</v>
       </c>
-      <c r="D34" t="s">
-        <v>7</v>
+      <c r="D34" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -1041,8 +1046,8 @@
       <c r="C35">
         <v>100</v>
       </c>
-      <c r="D35" t="s">
-        <v>7</v>
+      <c r="D35" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E35">
         <v>3</v>
@@ -1058,8 +1063,8 @@
       <c r="C36">
         <v>75</v>
       </c>
-      <c r="D36" t="s">
-        <v>7</v>
+      <c r="D36" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E36">
         <v>3</v>
@@ -1075,8 +1080,8 @@
       <c r="C37">
         <v>110</v>
       </c>
-      <c r="D37" t="s">
-        <v>7</v>
+      <c r="D37" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -1092,8 +1097,8 @@
       <c r="C38">
         <v>110</v>
       </c>
-      <c r="D38" t="s">
-        <v>7</v>
+      <c r="D38" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E38">
         <v>3</v>
@@ -1109,8 +1114,8 @@
       <c r="C39">
         <v>60</v>
       </c>
-      <c r="D39" t="s">
-        <v>7</v>
+      <c r="D39" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E39">
         <v>3</v>
@@ -1126,8 +1131,8 @@
       <c r="C40">
         <v>80</v>
       </c>
-      <c r="D40" t="s">
-        <v>7</v>
+      <c r="D40" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E40">
         <v>3</v>
@@ -1143,8 +1148,8 @@
       <c r="C41">
         <v>65</v>
       </c>
-      <c r="D41" t="s">
-        <v>7</v>
+      <c r="D41" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E41">
         <v>3</v>
@@ -1160,8 +1165,8 @@
       <c r="C42">
         <v>100</v>
       </c>
-      <c r="D42" t="s">
-        <v>7</v>
+      <c r="D42" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E42">
         <v>3</v>
@@ -1177,8 +1182,8 @@
       <c r="C43">
         <v>40</v>
       </c>
-      <c r="D43" t="s">
-        <v>7</v>
+      <c r="D43" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -1194,8 +1199,8 @@
       <c r="C44">
         <v>85</v>
       </c>
-      <c r="D44" t="s">
-        <v>7</v>
+      <c r="D44" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E44">
         <v>2</v>
@@ -1211,8 +1216,8 @@
       <c r="C45">
         <v>100</v>
       </c>
-      <c r="D45" t="s">
-        <v>7</v>
+      <c r="D45" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E45">
         <v>3</v>
@@ -1228,8 +1233,8 @@
       <c r="C46">
         <v>100</v>
       </c>
-      <c r="D46" t="s">
-        <v>7</v>
+      <c r="D46" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E46">
         <v>3</v>
@@ -1245,8 +1250,8 @@
       <c r="C47">
         <v>65</v>
       </c>
-      <c r="D47" t="s">
-        <v>7</v>
+      <c r="D47" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E47">
         <v>3</v>
@@ -1262,8 +1267,8 @@
       <c r="C48">
         <v>100</v>
       </c>
-      <c r="D48" t="s">
-        <v>7</v>
+      <c r="D48" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -1279,8 +1284,8 @@
       <c r="C49">
         <v>150</v>
       </c>
-      <c r="D49" t="s">
-        <v>7</v>
+      <c r="D49" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E49">
         <v>2</v>
@@ -1296,8 +1301,8 @@
       <c r="C50">
         <v>150</v>
       </c>
-      <c r="D50" t="s">
-        <v>7</v>
+      <c r="D50" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E50">
         <v>3</v>
@@ -1313,8 +1318,8 @@
       <c r="C51">
         <v>60</v>
       </c>
-      <c r="D51" t="s">
-        <v>7</v>
+      <c r="D51" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E51">
         <v>2</v>
@@ -1330,8 +1335,8 @@
       <c r="C52">
         <v>50</v>
       </c>
-      <c r="D52" t="s">
-        <v>7</v>
+      <c r="D52" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E52">
         <v>2</v>
@@ -1347,8 +1352,8 @@
       <c r="C53">
         <v>100</v>
       </c>
-      <c r="D53" t="s">
-        <v>7</v>
+      <c r="D53" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E53">
         <v>3</v>
@@ -1364,8 +1369,8 @@
       <c r="C54">
         <v>100</v>
       </c>
-      <c r="D54" t="s">
-        <v>7</v>
+      <c r="D54" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E54">
         <v>3</v>
@@ -1381,8 +1386,8 @@
       <c r="C55">
         <v>150</v>
       </c>
-      <c r="D55" t="s">
-        <v>7</v>
+      <c r="D55" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E55">
         <v>2</v>
@@ -1398,8 +1403,8 @@
       <c r="C56">
         <v>135</v>
       </c>
-      <c r="D56" t="s">
-        <v>7</v>
+      <c r="D56" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -1415,8 +1420,8 @@
       <c r="C57">
         <v>85</v>
       </c>
-      <c r="D57" t="s">
-        <v>7</v>
+      <c r="D57" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E57">
         <v>2</v>
@@ -1432,8 +1437,8 @@
       <c r="C58">
         <v>45</v>
       </c>
-      <c r="D58" t="s">
-        <v>7</v>
+      <c r="D58" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E58">
         <v>3</v>
@@ -1449,8 +1454,8 @@
       <c r="C59">
         <v>100</v>
       </c>
-      <c r="D59" t="s">
-        <v>7</v>
+      <c r="D59" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E59">
         <v>3</v>
@@ -1466,8 +1471,8 @@
       <c r="C60">
         <v>100</v>
       </c>
-      <c r="D60" t="s">
-        <v>7</v>
+      <c r="D60" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E60">
         <v>3</v>
@@ -1483,8 +1488,8 @@
       <c r="C61">
         <v>100</v>
       </c>
-      <c r="D61" t="s">
-        <v>7</v>
+      <c r="D61" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E61">
         <v>3</v>
@@ -1500,8 +1505,8 @@
       <c r="C62">
         <v>85</v>
       </c>
-      <c r="D62" t="s">
-        <v>7</v>
+      <c r="D62" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E62">
         <v>3</v>
@@ -1517,8 +1522,8 @@
       <c r="C63">
         <v>180</v>
       </c>
-      <c r="D63" t="s">
-        <v>8</v>
+      <c r="D63" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -1534,8 +1539,8 @@
       <c r="C64">
         <v>180</v>
       </c>
-      <c r="D64" t="s">
-        <v>8</v>
+      <c r="D64" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -1551,8 +1556,8 @@
       <c r="C65">
         <v>150</v>
       </c>
-      <c r="D65" t="s">
-        <v>8</v>
+      <c r="D65" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -1568,8 +1573,8 @@
       <c r="C66">
         <v>130</v>
       </c>
-      <c r="D66" t="s">
-        <v>8</v>
+      <c r="D66" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E66">
         <v>3</v>
@@ -1585,8 +1590,8 @@
       <c r="C67">
         <v>50</v>
       </c>
-      <c r="D67" t="s">
-        <v>8</v>
+      <c r="D67" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E67">
         <v>2</v>
@@ -1602,8 +1607,8 @@
       <c r="C68">
         <v>75</v>
       </c>
-      <c r="D68" t="s">
-        <v>8</v>
+      <c r="D68" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E68">
         <v>3</v>
@@ -1614,13 +1619,13 @@
         <v>36.367321843348002</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C69">
         <v>80</v>
       </c>
-      <c r="D69" t="s">
-        <v>8</v>
+      <c r="D69" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E69">
         <v>2</v>
@@ -1636,8 +1641,8 @@
       <c r="C70">
         <v>45</v>
       </c>
-      <c r="D70" t="s">
-        <v>8</v>
+      <c r="D70" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E70">
         <v>3</v>
@@ -1653,8 +1658,8 @@
       <c r="C71">
         <v>150</v>
       </c>
-      <c r="D71" t="s">
-        <v>8</v>
+      <c r="D71" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -1670,8 +1675,8 @@
       <c r="C72">
         <v>75</v>
       </c>
-      <c r="D72" t="s">
-        <v>8</v>
+      <c r="D72" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E72">
         <v>3</v>
@@ -1687,8 +1692,8 @@
       <c r="C73">
         <v>85</v>
       </c>
-      <c r="D73" t="s">
-        <v>8</v>
+      <c r="D73" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E73">
         <v>1</v>
@@ -1704,8 +1709,8 @@
       <c r="C74">
         <v>120</v>
       </c>
-      <c r="D74" t="s">
-        <v>8</v>
+      <c r="D74" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E74">
         <v>2</v>
@@ -1721,8 +1726,8 @@
       <c r="C75">
         <v>220</v>
       </c>
-      <c r="D75" t="s">
-        <v>8</v>
+      <c r="D75" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -1738,8 +1743,8 @@
       <c r="C76">
         <v>90</v>
       </c>
-      <c r="D76" t="s">
-        <v>8</v>
+      <c r="D76" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E76">
         <v>3</v>
@@ -1755,8 +1760,8 @@
       <c r="C77">
         <v>55</v>
       </c>
-      <c r="D77" t="s">
-        <v>8</v>
+      <c r="D77" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -1772,8 +1777,8 @@
       <c r="C78">
         <v>69</v>
       </c>
-      <c r="D78" t="s">
-        <v>8</v>
+      <c r="D78" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E78">
         <v>1</v>
@@ -1789,8 +1794,8 @@
       <c r="C79">
         <v>100</v>
       </c>
-      <c r="D79" t="s">
-        <v>8</v>
+      <c r="D79" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E79">
         <v>2</v>
@@ -1806,8 +1811,8 @@
       <c r="C80">
         <v>70</v>
       </c>
-      <c r="D80" t="s">
-        <v>8</v>
+      <c r="D80" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E80">
         <v>3</v>
@@ -1823,8 +1828,8 @@
       <c r="C81">
         <v>120</v>
       </c>
-      <c r="D81" t="s">
-        <v>8</v>
+      <c r="D81" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E81">
         <v>2</v>
@@ -1840,8 +1845,8 @@
       <c r="C82">
         <v>45</v>
       </c>
-      <c r="D82" t="s">
-        <v>8</v>
+      <c r="D82" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -1857,8 +1862,8 @@
       <c r="C83">
         <v>180</v>
       </c>
-      <c r="D83" t="s">
-        <v>8</v>
+      <c r="D83" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E83">
         <v>1</v>

</xml_diff>

<commit_message>
✨Feat : Create coordinate data
남은 작업 : 대학 기준 남, 남서, 서
</commit_message>
<xml_diff>
--- a/Documents/CrimePoint_within3km.xlsx
+++ b/Documents/CrimePoint_within3km.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seojiung/Documents/GitHub/DisabilityCrimeNavigator/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimdoo-young/#ConnectFolder/DisabilityCrimeNavigator/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA9E86F-CEB3-6D4E-9982-42CE86C7A7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D378DF-3DAE-C54F-A9A4-08002B08421A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{53916054-8B8C-4E74-BC5F-10B546F4D0E4}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" xr2:uid="{53916054-8B8C-4E74-BC5F-10B546F4D0E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="10">
   <si>
     <t>위도</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,7 +75,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +103,12 @@
       <color rgb="FFC77DBB"/>
       <name val="JetBrains Mono"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -126,7 +132,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -134,6 +140,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -450,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E8108C-04BD-2A42-96C4-40717F420405}">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1869,9 +1878,736 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="20">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
+    <row r="84" spans="1:5">
+      <c r="A84" s="3">
+        <v>36.362742345954402</v>
+      </c>
+      <c r="B84" s="3">
+        <v>127.418209237589</v>
+      </c>
+      <c r="C84">
+        <v>35</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="3">
+        <v>36.363813662847399</v>
+      </c>
+      <c r="B85" s="3">
+        <v>127.415376824869</v>
+      </c>
+      <c r="C85">
+        <v>40</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="3">
+        <v>36.363433519831602</v>
+      </c>
+      <c r="B86" s="3">
+        <v>127.413510007395</v>
+      </c>
+      <c r="C86">
+        <v>55</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="3">
+        <v>36.365126869886197</v>
+      </c>
+      <c r="B87" s="3">
+        <v>127.41374067737</v>
+      </c>
+      <c r="C87">
+        <v>70</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="3">
+        <v>36.365360134607997</v>
+      </c>
+      <c r="B88" s="3">
+        <v>127.411391062273</v>
+      </c>
+      <c r="C88">
+        <v>70</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="3">
+        <v>36.358344608378601</v>
+      </c>
+      <c r="B89" s="3">
+        <v>127.432623428835</v>
+      </c>
+      <c r="C89">
+        <v>60</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="3">
+        <v>36.356772076083701</v>
+      </c>
+      <c r="B90" s="3">
+        <v>127.43125550223699</v>
+      </c>
+      <c r="C90">
+        <v>100</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="3">
+        <v>36.356737514577603</v>
+      </c>
+      <c r="B91" s="3">
+        <v>127.427232188715</v>
+      </c>
+      <c r="C91">
+        <v>65</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="3">
+        <v>36.358197724839101</v>
+      </c>
+      <c r="B92" s="3">
+        <v>127.426556272043</v>
+      </c>
+      <c r="C92">
+        <v>130</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="3">
+        <v>36.356772076083701</v>
+      </c>
+      <c r="B93" s="3">
+        <v>127.431244773401</v>
+      </c>
+      <c r="C93">
+        <v>60</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="3">
+        <v>36.355527852194797</v>
+      </c>
+      <c r="B94" s="3">
+        <v>127.431486172213</v>
+      </c>
+      <c r="C94">
+        <v>100</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="3">
+        <v>36.354274967766202</v>
+      </c>
+      <c r="B95" s="3">
+        <v>127.43241958095</v>
+      </c>
+      <c r="C95">
+        <v>150</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="3">
+        <v>36.353937981616497</v>
+      </c>
+      <c r="B96" s="3">
+        <v>127.43132523967201</v>
+      </c>
+      <c r="C96">
+        <v>100</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="3">
+        <v>36.3531948787979</v>
+      </c>
+      <c r="B97" s="3">
+        <v>127.43029527141</v>
+      </c>
+      <c r="C97">
+        <v>100</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="3">
+        <v>36.3521061339518</v>
+      </c>
+      <c r="B98" s="3">
+        <v>127.430166525377</v>
+      </c>
+      <c r="C98">
+        <v>100</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="3">
+        <v>36.350870476513101</v>
+      </c>
+      <c r="B99" s="3">
+        <v>127.43005923701701</v>
+      </c>
+      <c r="C99">
+        <v>45</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="3">
+        <v>36.351112424968299</v>
+      </c>
+      <c r="B100" s="3">
+        <v>127.42660174271199</v>
+      </c>
+      <c r="C100">
+        <v>200</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="3">
+        <v>36.350524834558499</v>
+      </c>
+      <c r="B101" s="3">
+        <v>127.43000278374301</v>
+      </c>
+      <c r="C101">
+        <v>100</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="3">
+        <v>36.349384205221099</v>
+      </c>
+      <c r="B102" s="3">
+        <v>127.431150769201</v>
+      </c>
+      <c r="C102">
+        <v>100</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="3">
+        <v>36.3488052430274</v>
+      </c>
+      <c r="B103" s="3">
+        <v>127.43098983666</v>
+      </c>
+      <c r="C103">
+        <v>80</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="3">
+        <v>36.348468233200997</v>
+      </c>
+      <c r="B104" s="3">
+        <v>127.434744929281</v>
+      </c>
+      <c r="C104">
+        <v>100</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="3">
+        <v>36.348891655568501</v>
+      </c>
+      <c r="B105" s="3">
+        <v>127.43314633270801</v>
+      </c>
+      <c r="C105">
+        <v>50</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="3">
+        <v>36.349798981459102</v>
+      </c>
+      <c r="B106" s="3">
+        <v>127.437888478247</v>
+      </c>
+      <c r="C106">
+        <v>75</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="3">
+        <v>36.351432141416502</v>
+      </c>
+      <c r="B107" s="3">
+        <v>127.43682632347701</v>
+      </c>
+      <c r="C107">
+        <v>60</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="3">
+        <v>36.352486332294902</v>
+      </c>
+      <c r="B108" s="3">
+        <v>127.436461543051</v>
+      </c>
+      <c r="C108">
+        <v>120</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="20">
+      <c r="A109" s="1">
+        <v>36.350835863543097</v>
+      </c>
+      <c r="B109" s="1">
+        <v>127.44708888764301</v>
+      </c>
+      <c r="C109">
+        <v>35</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="20">
+      <c r="A110" s="1">
+        <v>36.354168813452098</v>
+      </c>
+      <c r="B110" s="1">
+        <v>127.44985973999199</v>
+      </c>
+      <c r="C110">
+        <v>55</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="20">
+      <c r="A111" s="1">
+        <v>36.356062172304398</v>
+      </c>
+      <c r="B111" s="1">
+        <v>127.452009732443</v>
+      </c>
+      <c r="C111">
+        <v>45</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E111">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="20">
+      <c r="A112" s="1">
+        <v>36.356206507972303</v>
+      </c>
+      <c r="B112" s="1">
+        <v>127.449581795304</v>
+      </c>
+      <c r="C112">
+        <v>40</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="20">
+      <c r="A113" s="1">
+        <v>36.349120371810699</v>
+      </c>
+      <c r="B113" s="1">
+        <v>127.451551847609</v>
+      </c>
+      <c r="C113">
+        <v>200</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="20">
+      <c r="A114" s="1">
+        <v>36.349607386296199</v>
+      </c>
+      <c r="B114" s="1">
+        <v>127.449059251905</v>
+      </c>
+      <c r="C114">
+        <v>25</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="20">
+      <c r="A115" s="1">
+        <v>36.3473797144309</v>
+      </c>
+      <c r="B115" s="1">
+        <v>127.451920553083</v>
+      </c>
+      <c r="C115">
+        <v>35</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="20">
+      <c r="A116" s="1">
+        <v>36.347011059349299</v>
+      </c>
+      <c r="B116" s="1">
+        <v>127.44931169914</v>
+      </c>
+      <c r="C116">
+        <v>40</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="20">
+      <c r="A117" s="1">
+        <v>36.346275839354803</v>
+      </c>
+      <c r="B117" s="1">
+        <v>127.450711082293</v>
+      </c>
+      <c r="C117">
+        <v>30</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="20">
+      <c r="A118" s="1">
+        <v>36.346326081007398</v>
+      </c>
+      <c r="B118" s="1">
+        <v>127.451725088769</v>
+      </c>
+      <c r="C118">
+        <v>40</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="20">
+      <c r="A119" s="1">
+        <v>36.345036223363998</v>
+      </c>
+      <c r="B119" s="1">
+        <v>127.442404962629</v>
+      </c>
+      <c r="C119">
+        <v>50</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="20">
+      <c r="A120" s="1">
+        <v>36.344090134462697</v>
+      </c>
+      <c r="B120" s="1">
+        <v>127.442366192737</v>
+      </c>
+      <c r="C120">
+        <v>50</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="20">
+      <c r="A121" s="1">
+        <v>36.345930262467903</v>
+      </c>
+      <c r="B121" s="1">
+        <v>127.441897594102</v>
+      </c>
+      <c r="C121">
+        <v>50</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E121">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="20">
+      <c r="A122" s="1">
+        <v>36.346761588804398</v>
+      </c>
+      <c r="B122" s="1">
+        <v>127.44128960179999</v>
+      </c>
+      <c r="C122">
+        <v>50</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="20">
+      <c r="A123" s="1">
+        <v>36.347013237509401</v>
+      </c>
+      <c r="B123" s="1">
+        <v>127.43656772545501</v>
+      </c>
+      <c r="C123">
+        <v>50</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="20">
+      <c r="A124" s="1">
+        <v>36.344407518653099</v>
+      </c>
+      <c r="B124" s="1">
+        <v>127.434458957825</v>
+      </c>
+      <c r="C124">
+        <v>50</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="20">
+      <c r="A125" s="1">
+        <v>36.343558324910298</v>
+      </c>
+      <c r="B125" s="1">
+        <v>127.43503348739701</v>
+      </c>
+      <c r="C125">
+        <v>40</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="20">
+      <c r="A126" s="1">
+        <v>36.344223395003098</v>
+      </c>
+      <c r="B126" s="1">
+        <v>127.435527322639</v>
+      </c>
+      <c r="C126">
+        <v>20</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E126">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>